<commit_message>
A couple of addictions
</commit_message>
<xml_diff>
--- a/LTL Statistik.xlsx
+++ b/LTL Statistik.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d89bd5ff47ebf7c5/Documents/Github/LongTermEnvLogger/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="173" documentId="8_{8A4E7535-D9D0-CA43-9274-22CAB0D7301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6904F057-51BF-5049-A941-9DB72B4C4F5B}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="8_{8A4E7535-D9D0-CA43-9274-22CAB0D7301D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B9EA288B-DCAF-2141-AE2F-2D0C8CBE0EAB}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="5300" windowWidth="38400" windowHeight="23500" activeTab="3" xr2:uid="{EFA3F9BA-CB12-BF40-9697-4468815D2522}"/>
+    <workbookView minimized="1" xWindow="51200" yWindow="5300" windowWidth="38400" windowHeight="23500" activeTab="4" xr2:uid="{EFA3F9BA-CB12-BF40-9697-4468815D2522}"/>
   </bookViews>
   <sheets>
     <sheet name="Statistik" sheetId="2" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="4" r:id="rId2"/>
     <sheet name="Tabelle1" sheetId="3" r:id="rId3"/>
     <sheet name="E-Reihen" sheetId="1" r:id="rId4"/>
+    <sheet name="Spannungsteiler" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -166,7 +167,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -230,6 +231,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -33019,7 +33022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC069DF7-F8AB-AB49-8F38-DD3180601AC7}">
   <dimension ref="B2:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -34023,4 +34026,395 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE719A1E-1D5C-2E4C-9A78-573F7C41FE1C}">
+  <dimension ref="D6:G49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="6" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>3.16</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ref="E6:E10" si="0">(4.2*10)/(D6*10+10)</f>
+        <v>1.0096153846153846</v>
+      </c>
+      <c r="G6">
+        <f>E6*1.01</f>
+        <v>1.0197115384615385</v>
+      </c>
+    </row>
+    <row r="7" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>3.24</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.99056603773584895</v>
+      </c>
+      <c r="F7" s="25"/>
+      <c r="G7">
+        <f>E7*1.01</f>
+        <v>1.0004716981132074</v>
+      </c>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>3.32</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>0.97222222222222232</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ref="G8:G19" si="1">E8*1.01</f>
+        <v>0.98194444444444451</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>3.48</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>0.93750000000000011</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.94687500000000013</v>
+      </c>
+    </row>
+    <row r="10" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>3.57</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>0.91903719912472659</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>0.92822757111597387</v>
+      </c>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>3.65</v>
+      </c>
+      <c r="E11">
+        <f>(4.2*10)/(D11*10+10)</f>
+        <v>0.90322580645161288</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>0.91225806451612901</v>
+      </c>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>3.74</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:E19" si="2">(4.2*10)/(D12*10+10)</f>
+        <v>0.88607594936708856</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>0.89493670886075949</v>
+      </c>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>3.83</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0.86956521739130443</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>0.87826086956521754</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>3.92</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>0.85365853658536583</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>0.8621951219512195</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>4.0199999999999996</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="2"/>
+        <v>0.8366533864541833</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>0.84501992031872519</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="2"/>
+        <v>1.05</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>1.0605</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>3.3</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="2"/>
+        <v>0.97674418604651159</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>0.98651162790697666</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>3.9</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="2"/>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0.86571428571428566</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>4.3</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="2"/>
+        <v>0.79245283018867929</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0.80037735849056613</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D27" s="26">
+        <v>0.32951388888888888</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D28" s="26">
+        <v>0.3300925925925926</v>
+      </c>
+      <c r="E28" s="26">
+        <f>D28-D27</f>
+        <v>5.7870370370372015E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D29" s="26">
+        <v>0.33055555555555555</v>
+      </c>
+      <c r="E29" s="26">
+        <f>D29-D28</f>
+        <v>4.6296296296294281E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D30" s="26">
+        <v>0.33113425925925927</v>
+      </c>
+      <c r="E30" s="26">
+        <f>D30-D29</f>
+        <v>5.7870370370372015E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D31" s="26">
+        <v>0.33171296296296299</v>
+      </c>
+      <c r="E31" s="26">
+        <f>D31-D30</f>
+        <v>5.7870370370372015E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.2">
+      <c r="D32" s="26">
+        <v>0.33229166666666665</v>
+      </c>
+      <c r="E32" s="26">
+        <f>D32-D31</f>
+        <v>5.7870370370366464E-4</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E33" s="26"/>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D34" s="26">
+        <v>0.32557870370370373</v>
+      </c>
+      <c r="E34" s="26"/>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D35" s="26">
+        <v>0.32743055555555556</v>
+      </c>
+      <c r="E35" s="26">
+        <f t="shared" ref="E33:E49" si="3">D35-D34</f>
+        <v>1.8518518518518268E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D36" s="26">
+        <v>0.32916666666666666</v>
+      </c>
+      <c r="E36" s="26">
+        <f t="shared" si="3"/>
+        <v>1.7361111111111049E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D37" s="26">
+        <v>0.33101851851851855</v>
+      </c>
+      <c r="E37" s="26">
+        <f t="shared" si="3"/>
+        <v>1.8518518518518823E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D38" s="26">
+        <v>0.33275462962962965</v>
+      </c>
+      <c r="E38" s="26">
+        <f t="shared" si="3"/>
+        <v>1.7361111111111049E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D39" s="26">
+        <v>0.33460648148148148</v>
+      </c>
+      <c r="E39" s="26">
+        <f t="shared" si="3"/>
+        <v>1.8518518518518268E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D40" s="26">
+        <v>0.33634259259259258</v>
+      </c>
+      <c r="E40" s="26">
+        <f t="shared" si="3"/>
+        <v>1.7361111111111049E-3</v>
+      </c>
+      <c r="F40" s="26">
+        <f>AVERAGE(E35:E40)</f>
+        <v>1.7939814814814752E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="E41" s="26"/>
+    </row>
+    <row r="42" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D42" s="26">
+        <v>0.29895833333333333</v>
+      </c>
+      <c r="E42" s="26"/>
+    </row>
+    <row r="43" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D43" s="26">
+        <v>0.30324074074074076</v>
+      </c>
+      <c r="E43" s="26">
+        <f t="shared" si="3"/>
+        <v>4.2824074074074292E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D44" s="26">
+        <v>0.30763888888888891</v>
+      </c>
+      <c r="E44" s="26">
+        <f t="shared" si="3"/>
+        <v>4.398148148148151E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D45" s="26">
+        <v>0.31192129629629628</v>
+      </c>
+      <c r="E45" s="26">
+        <f t="shared" si="3"/>
+        <v>4.2824074074073737E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D46" s="26">
+        <v>0.31620370370370371</v>
+      </c>
+      <c r="E46" s="26">
+        <f t="shared" si="3"/>
+        <v>4.2824074074074292E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D47" s="26">
+        <v>0.32060185185185186</v>
+      </c>
+      <c r="E47" s="26">
+        <f t="shared" si="3"/>
+        <v>4.398148148148151E-3</v>
+      </c>
+      <c r="F47" s="26">
+        <f>AVERAGE(E43:E47)</f>
+        <v>4.328703703703707E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D48" s="26">
+        <v>0.32916666666666666</v>
+      </c>
+      <c r="E48" s="26">
+        <f t="shared" si="3"/>
+        <v>8.5648148148148029E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="4:5" x14ac:dyDescent="0.2">
+      <c r="D49" s="26">
+        <v>0.33356481481481481</v>
+      </c>
+      <c r="E49" s="26">
+        <f t="shared" si="3"/>
+        <v>4.398148148148151E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>